<commit_message>
add multi regression model
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -383,6 +383,11 @@
           <t>MedianAge</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total_beds_per1000</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -406,6 +411,9 @@
       <c r="E2">
         <v>39.2</v>
       </c>
+      <c r="F2">
+        <v>3.06</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -429,6 +437,9 @@
       <c r="E3">
         <v>34.6</v>
       </c>
+      <c r="F3">
+        <v>2.17</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -452,6 +463,9 @@
       <c r="E4">
         <v>37.9</v>
       </c>
+      <c r="F4">
+        <v>1.99</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -475,6 +489,9 @@
       <c r="E5">
         <v>38.3</v>
       </c>
+      <c r="F5">
+        <v>3.16</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -498,6 +515,9 @@
       <c r="E6">
         <v>36.7</v>
       </c>
+      <c r="F6">
+        <v>1.84</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -521,6 +541,9 @@
       <c r="E7">
         <v>36.9</v>
       </c>
+      <c r="F7">
+        <v>1.91</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -544,6 +567,9 @@
       <c r="E8">
         <v>41.1</v>
       </c>
+      <c r="F8">
+        <v>2.09</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -567,6 +593,9 @@
       <c r="E9">
         <v>41</v>
       </c>
+      <c r="F9">
+        <v>2.2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -590,6 +619,9 @@
       <c r="E10">
         <v>42.2</v>
       </c>
+      <c r="F10">
+        <v>2.55</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -613,6 +645,9 @@
       <c r="E11">
         <v>36.9</v>
       </c>
+      <c r="F11">
+        <v>2.34</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -636,6 +671,9 @@
       <c r="E12">
         <v>39.4</v>
       </c>
+      <c r="F12">
+        <v>1.85</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -659,6 +697,9 @@
       <c r="E13">
         <v>36.6</v>
       </c>
+      <c r="F13">
+        <v>1.91</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -682,6 +723,9 @@
       <c r="E14">
         <v>38.3</v>
       </c>
+      <c r="F14">
+        <v>2.49</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -705,6 +749,9 @@
       <c r="E15">
         <v>37.8</v>
       </c>
+      <c r="F15">
+        <v>2.71</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -728,6 +775,9 @@
       <c r="E16">
         <v>38.3</v>
       </c>
+      <c r="F16">
+        <v>2.85</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -751,6 +801,9 @@
       <c r="E17">
         <v>36.9</v>
       </c>
+      <c r="F17">
+        <v>3.19</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -774,6 +827,9 @@
       <c r="E18">
         <v>39</v>
       </c>
+      <c r="F18">
+        <v>3.17</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -797,6 +853,9 @@
       <c r="E19">
         <v>37.2</v>
       </c>
+      <c r="F19">
+        <v>3.25</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -820,6 +879,9 @@
       <c r="E20">
         <v>44.8</v>
       </c>
+      <c r="F20">
+        <v>2.56</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -843,6 +905,9 @@
       <c r="E21">
         <v>38.8</v>
       </c>
+      <c r="F21">
+        <v>1.82</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -866,6 +931,9 @@
       <c r="E22">
         <v>39.6</v>
       </c>
+      <c r="F22">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -889,6 +957,9 @@
       <c r="E23">
         <v>39.8</v>
       </c>
+      <c r="F23">
+        <v>2.43</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -912,6 +983,9 @@
       <c r="E24">
         <v>38.1</v>
       </c>
+      <c r="F24">
+        <v>2.43</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -935,6 +1009,9 @@
       <c r="E25">
         <v>37.7</v>
       </c>
+      <c r="F25">
+        <v>3.99</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -958,6 +1035,9 @@
       <c r="E26">
         <v>38.7</v>
       </c>
+      <c r="F26">
+        <v>3.01</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -981,6 +1061,9 @@
       <c r="E27">
         <v>40.1</v>
       </c>
+      <c r="F27">
+        <v>3.46</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1004,6 +1087,9 @@
       <c r="E28">
         <v>36.6</v>
       </c>
+      <c r="F28">
+        <v>3.38</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1027,6 +1113,9 @@
       <c r="E29">
         <v>38.2</v>
       </c>
+      <c r="F29">
+        <v>2.08</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1050,6 +1139,9 @@
       <c r="E30">
         <v>43</v>
       </c>
+      <c r="F30">
+        <v>2.04</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1073,6 +1165,9 @@
       <c r="E31">
         <v>40</v>
       </c>
+      <c r="F31">
+        <v>2.36</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1096,6 +1191,9 @@
       <c r="E32">
         <v>38.1</v>
       </c>
+      <c r="F32">
+        <v>1.79</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1119,6 +1217,9 @@
       <c r="E33">
         <v>39</v>
       </c>
+      <c r="F33">
+        <v>2.52</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1142,6 +1243,9 @@
       <c r="E34">
         <v>38.9</v>
       </c>
+      <c r="F34">
+        <v>2.08</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1165,6 +1269,9 @@
       <c r="E35">
         <v>35.2</v>
       </c>
+      <c r="F35">
+        <v>4.31</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1188,6 +1295,9 @@
       <c r="E36">
         <v>39.5</v>
       </c>
+      <c r="F36">
+        <v>2.73</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1211,6 +1321,9 @@
       <c r="E37">
         <v>36.7</v>
       </c>
+      <c r="F37">
+        <v>2.81</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1234,6 +1347,9 @@
       <c r="E38">
         <v>39.5</v>
       </c>
+      <c r="F38">
+        <v>1.64</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1257,6 +1373,9 @@
       <c r="E39">
         <v>40.9</v>
       </c>
+      <c r="F39">
+        <v>2.73</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1280,6 +1399,9 @@
       <c r="E40">
         <v>40</v>
       </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1303,6 +1425,9 @@
       <c r="E41">
         <v>39.7</v>
       </c>
+      <c r="F41">
+        <v>2.19</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1326,6 +1451,9 @@
       <c r="E42">
         <v>37.2</v>
       </c>
+      <c r="F42">
+        <v>4.82</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1349,6 +1477,9 @@
       <c r="E43">
         <v>38.8</v>
       </c>
+      <c r="F43">
+        <v>2.77</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1372,6 +1503,9 @@
       <c r="E44">
         <v>34.8</v>
       </c>
+      <c r="F44">
+        <v>2.28</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1395,6 +1529,9 @@
       <c r="E45">
         <v>31.1</v>
       </c>
+      <c r="F45">
+        <v>1.8</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1418,6 +1555,9 @@
       <c r="E46">
         <v>42.8</v>
       </c>
+      <c r="F46">
+        <v>2.08</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1441,6 +1581,9 @@
       <c r="E47">
         <v>38.4</v>
       </c>
+      <c r="F47">
+        <v>2.1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1464,6 +1607,9 @@
       <c r="E48">
         <v>37.8</v>
       </c>
+      <c r="F48">
+        <v>1.58</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1487,6 +1633,9 @@
       <c r="E49">
         <v>42.7</v>
       </c>
+      <c r="F49">
+        <v>3.52</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1510,6 +1659,9 @@
       <c r="E50">
         <v>39.6</v>
       </c>
+      <c r="F50">
+        <v>2.08</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1532,6 +1684,9 @@
       </c>
       <c r="E51">
         <v>38</v>
+      </c>
+      <c r="F51">
+        <v>3.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>